<commit_message>
Importing spreadsheet now gracefully handles Owners with no last name
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/first_name_only.xlsx
+++ b/spec/fixtures/files/first_name_only.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="13410"/>
   </bookViews>
   <sheets>
-    <sheet name="AppendList" sheetId="1" r:id="rId3"/>
+    <sheet name="AppendList" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Serial No</t>
   </si>
@@ -106,11 +109,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -118,11 +118,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <sz val="15"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
@@ -283,52 +278,50 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="19" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="19" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -338,56 +331,388 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ff4f81bd"/>
-      <rgbColor rgb="ff7f7f7f"/>
-      <rgbColor rgb="fff2dbdb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FF4F81BD"/>
+      <rgbColor rgb="FF7F7F7F"/>
+      <rgbColor rgb="FFF2DBDB"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:R3"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.59765625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.8984375" style="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.75" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6.625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="6.625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="6.625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="6.625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="6.625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="6.625" style="1" customWidth="1"/>
-    <col min="19" max="256" width="6.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.59765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.59765625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.69921875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.8984375" style="1" customWidth="1"/>
+    <col min="8" max="11" width="6.59765625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11" style="1" customWidth="1"/>
+    <col min="13" max="256" width="6.59765625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -407,73 +732,73 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
     </row>
-    <row r="2" ht="17" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s" s="5">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s" s="5">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s" s="3">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s" s="3">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s" s="3">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s" s="3">
+      <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s" s="3">
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" t="s" s="3">
+      <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" t="s" s="3">
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" t="s" s="3">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" t="s" s="3">
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" t="s" s="3">
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P2" t="s" s="3">
+      <c r="P2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" t="s" s="3">
+      <c r="Q2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R2" t="s" s="3">
+      <c r="R2" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" ht="17" customHeight="1">
-      <c r="A3" t="s" s="6">
+    <row r="3" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s" s="7">
+      <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s" s="8">
+      <c r="C3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s" s="8">
+      <c r="D3" s="8" t="s">
         <v>21</v>
       </c>
       <c r="E3" s="9">
@@ -486,36 +811,36 @@
       <c r="H3" s="12">
         <v>0.93</v>
       </c>
-      <c r="I3" t="s" s="6">
+      <c r="I3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J3" t="s" s="6">
+      <c r="J3" s="6" t="s">
         <v>23</v>
       </c>
       <c r="K3" s="13"/>
-      <c r="L3" t="s" s="6">
+      <c r="L3" s="6" t="s">
         <v>24</v>
       </c>
       <c r="M3" s="13"/>
-      <c r="N3" t="s" s="6">
+      <c r="N3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O3" t="s" s="6">
+      <c r="O3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="P3" t="s" s="6">
+      <c r="P3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" t="s" s="6">
+      <c r="Q3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="R3" t="s" s="6">
+      <c r="R3" s="6" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
+  <pageSetup orientation="landscape"/>
   <headerFooter>
     <oddFooter>&amp;"Helvetica,Regular"&amp;11&amp;P</oddFooter>
   </headerFooter>

</xml_diff>